<commit_message>
update code print number of Page
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP008_ComparingSalaryBonusTemp.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP008_ComparingSalaryBonusTemp.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$R$128</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$55</definedName>
     <definedName name="RangeChildRaising">Sheet1!#REF!</definedName>
     <definedName name="RangeChildRaisingManual">Sheet1!$A$9:$A$9</definedName>
     <definedName name="RangeDeliveryNoticeAmount">Sheet1!#REF!</definedName>
@@ -148,6 +148,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -161,9 +164,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R201"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="50" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:H60"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -516,26 +516,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="7"/>
@@ -546,28 +546,28 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
@@ -580,14 +580,14 @@
       <c r="R3" s="12"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -600,82 +600,82 @@
       <c r="R4" s="12"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
     </row>
     <row r="8" spans="1:18" ht="21" customHeight="1">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -689,13 +689,13 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -709,13 +709,13 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
       <c r="A10" s="6"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -729,13 +729,13 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
       <c r="A11" s="6"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -749,13 +749,13 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
       <c r="A12" s="6"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -769,13 +769,13 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
       <c r="A13" s="6"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -789,13 +789,13 @@
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -809,13 +809,13 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1">
       <c r="A15" s="6"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -889,13 +889,13 @@
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1">
       <c r="A19" s="6"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -909,13 +909,13 @@
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1">
       <c r="A20" s="6"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -929,13 +929,13 @@
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1">
       <c r="A21" s="6"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -949,13 +949,13 @@
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1">
       <c r="A22" s="6"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -969,13 +969,13 @@
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1">
       <c r="A23" s="6"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
@@ -990,12 +990,12 @@
     <row r="24" spans="1:18" ht="15" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="13"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
@@ -1010,12 +1010,12 @@
     <row r="25" spans="1:18" ht="15" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="13"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -1030,12 +1030,12 @@
     <row r="26" spans="1:18">
       <c r="A26" s="10"/>
       <c r="B26" s="13"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -1050,12 +1050,12 @@
     <row r="27" spans="1:18">
       <c r="A27" s="10"/>
       <c r="B27" s="13"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
@@ -1070,12 +1070,12 @@
     <row r="28" spans="1:18">
       <c r="A28" s="10"/>
       <c r="B28" s="13"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
@@ -1090,12 +1090,12 @@
     <row r="29" spans="1:18">
       <c r="A29" s="10"/>
       <c r="B29" s="13"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -1110,12 +1110,12 @@
     <row r="30" spans="1:18">
       <c r="A30" s="10"/>
       <c r="B30" s="13"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
@@ -1130,12 +1130,12 @@
     <row r="31" spans="1:18">
       <c r="A31" s="10"/>
       <c r="B31" s="13"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
@@ -1150,12 +1150,12 @@
     <row r="32" spans="1:18">
       <c r="A32" s="10"/>
       <c r="B32" s="13"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -1170,12 +1170,12 @@
     <row r="33" spans="1:18">
       <c r="A33" s="10"/>
       <c r="B33" s="13"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -1190,12 +1190,12 @@
     <row r="34" spans="1:18">
       <c r="A34" s="10"/>
       <c r="B34" s="13"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -1210,12 +1210,12 @@
     <row r="35" spans="1:18">
       <c r="A35" s="10"/>
       <c r="B35" s="13"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
@@ -1230,12 +1230,12 @@
     <row r="36" spans="1:18">
       <c r="A36" s="10"/>
       <c r="B36" s="13"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
@@ -1250,12 +1250,12 @@
     <row r="37" spans="1:18">
       <c r="A37" s="10"/>
       <c r="B37" s="13"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -1270,12 +1270,12 @@
     <row r="38" spans="1:18">
       <c r="A38" s="10"/>
       <c r="B38" s="13"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -1290,12 +1290,12 @@
     <row r="39" spans="1:18">
       <c r="A39" s="10"/>
       <c r="B39" s="13"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -1310,12 +1310,12 @@
     <row r="40" spans="1:18">
       <c r="A40" s="10"/>
       <c r="B40" s="13"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -1330,12 +1330,12 @@
     <row r="41" spans="1:18">
       <c r="A41" s="10"/>
       <c r="B41" s="13"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
@@ -1350,12 +1350,12 @@
     <row r="42" spans="1:18">
       <c r="A42" s="10"/>
       <c r="B42" s="13"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
@@ -1370,12 +1370,12 @@
     <row r="43" spans="1:18">
       <c r="A43" s="10"/>
       <c r="B43" s="13"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
@@ -1390,12 +1390,12 @@
     <row r="44" spans="1:18">
       <c r="A44" s="10"/>
       <c r="B44" s="13"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -1410,12 +1410,12 @@
     <row r="45" spans="1:18">
       <c r="A45" s="10"/>
       <c r="B45" s="13"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -1430,12 +1430,12 @@
     <row r="46" spans="1:18">
       <c r="A46" s="10"/>
       <c r="B46" s="13"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -1450,12 +1450,12 @@
     <row r="47" spans="1:18">
       <c r="A47" s="10"/>
       <c r="B47" s="13"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -1470,12 +1470,12 @@
     <row r="48" spans="1:18">
       <c r="A48" s="10"/>
       <c r="B48" s="13"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -1490,12 +1490,12 @@
     <row r="49" spans="1:18">
       <c r="A49" s="10"/>
       <c r="B49" s="13"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -1510,12 +1510,12 @@
     <row r="50" spans="1:18">
       <c r="A50" s="10"/>
       <c r="B50" s="13"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -1530,12 +1530,12 @@
     <row r="51" spans="1:18">
       <c r="A51" s="10"/>
       <c r="B51" s="13"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -1550,12 +1550,12 @@
     <row r="52" spans="1:18">
       <c r="A52" s="10"/>
       <c r="B52" s="13"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -1570,12 +1570,12 @@
     <row r="53" spans="1:18">
       <c r="A53" s="10"/>
       <c r="B53" s="13"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -1590,12 +1590,12 @@
     <row r="54" spans="1:18">
       <c r="A54" s="10"/>
       <c r="B54" s="13"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -1610,12 +1610,12 @@
     <row r="55" spans="1:18">
       <c r="A55" s="10"/>
       <c r="B55" s="13"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -1630,12 +1630,12 @@
     <row r="56" spans="1:18">
       <c r="A56" s="10"/>
       <c r="B56" s="13"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -1650,12 +1650,12 @@
     <row r="57" spans="1:18">
       <c r="A57" s="10"/>
       <c r="B57" s="13"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
@@ -1670,12 +1670,12 @@
     <row r="58" spans="1:18">
       <c r="A58" s="10"/>
       <c r="B58" s="13"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="19"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
@@ -1690,12 +1690,12 @@
     <row r="59" spans="1:18">
       <c r="A59" s="10"/>
       <c r="B59" s="13"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -1710,12 +1710,12 @@
     <row r="60" spans="1:18">
       <c r="A60" s="10"/>
       <c r="B60" s="13"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>

</xml_diff>